<commit_message>
different sourceTSs show up in Tester.xlsm::Overview
</commit_message>
<xml_diff>
--- a/Config/50/TestSet50.xlsx
+++ b/Config/50/TestSet50.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>SimulId</t>
   </si>
@@ -110,6 +110,21 @@
   </si>
   <si>
     <t>trainDS2</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-0.xml  9044</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-1.xml  9044</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-2.xml  9044</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-3.xml  9044</t>
+  </si>
+  <si>
+    <t>Engine2</t>
   </si>
 </sst>
 </file>
@@ -582,23 +597,23 @@
         <v>#REF!</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C6&amp;".xml "&amp;$A6</f>
+        <f t="shared" ref="E6:E37" si="1">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C6&amp;".xml "&amp;$A6</f>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 10408</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" ref="F6:I25" si="2">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A6</f>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10408</v>
       </c>
       <c r="G6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10408</v>
       </c>
       <c r="H6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10408</v>
       </c>
       <c r="I6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10408</v>
       </c>
     </row>
@@ -617,23 +632,23 @@
         <v>#REF!</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C7&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 9428</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9428</v>
       </c>
       <c r="G7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9428</v>
       </c>
       <c r="H7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9428</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9428</v>
       </c>
     </row>
@@ -652,23 +667,23 @@
         <v>#REF!</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C8&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 7756</v>
       </c>
       <c r="F8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 7756</v>
       </c>
       <c r="G8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 7756</v>
       </c>
       <c r="H8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 7756</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 7756</v>
       </c>
     </row>
@@ -687,23 +702,23 @@
         <v>#REF!</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C9&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 232</v>
       </c>
       <c r="F9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 232</v>
       </c>
       <c r="G9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 232</v>
       </c>
       <c r="H9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 232</v>
       </c>
       <c r="I9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 232</v>
       </c>
     </row>
@@ -722,23 +737,23 @@
         <v>#REF!</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C10&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 10028</v>
       </c>
       <c r="F10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10028</v>
       </c>
       <c r="G10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10028</v>
       </c>
       <c r="H10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10028</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10028</v>
       </c>
     </row>
@@ -757,23 +772,23 @@
         <v>#REF!</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C11&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 10512</v>
       </c>
       <c r="F11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10512</v>
       </c>
       <c r="G11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10512</v>
       </c>
       <c r="H11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10512</v>
       </c>
       <c r="I11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10512</v>
       </c>
     </row>
@@ -792,23 +807,23 @@
         <v>#REF!</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C12&amp;".xml "&amp;$A12</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 2092</v>
       </c>
       <c r="F12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A12</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 2092</v>
       </c>
       <c r="G12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A12</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 2092</v>
       </c>
       <c r="H12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A12</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 2092</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A12</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 2092</v>
       </c>
     </row>
@@ -827,23 +842,23 @@
         <v>#REF!</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C13&amp;".xml "&amp;$A13</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 9084</v>
       </c>
       <c r="F13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A13</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9084</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A13</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9084</v>
       </c>
       <c r="H13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A13</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9084</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A13</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9084</v>
       </c>
     </row>
@@ -862,23 +877,23 @@
         <v>#REF!</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C14&amp;".xml "&amp;$A14</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 10020</v>
       </c>
       <c r="F14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A14</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10020</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A14</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10020</v>
       </c>
       <c r="H14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A14</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10020</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A14</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10020</v>
       </c>
     </row>
@@ -897,23 +912,23 @@
         <v>#REF!</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C15&amp;".xml "&amp;$A15</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 9252</v>
       </c>
       <c r="F15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A15</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9252</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A15</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9252</v>
       </c>
       <c r="H15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A15</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9252</v>
       </c>
       <c r="I15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A15</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9252</v>
       </c>
     </row>
@@ -932,23 +947,23 @@
         <v>#REF!</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C16&amp;".xml "&amp;$A16</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 9036</v>
       </c>
       <c r="F16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A16</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9036</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A16</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9036</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A16</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9036</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A16</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9036</v>
       </c>
     </row>
@@ -967,23 +982,23 @@
         <v>#REF!</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C17&amp;".xml "&amp;$A17</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 8356</v>
       </c>
       <c r="F17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A17</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 8356</v>
       </c>
       <c r="G17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A17</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 8356</v>
       </c>
       <c r="H17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A17</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 8356</v>
       </c>
       <c r="I17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A17</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 8356</v>
       </c>
     </row>
@@ -1002,23 +1017,23 @@
         <v>#REF!</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C18&amp;".xml "&amp;$A18</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 2035</v>
       </c>
       <c r="F18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A18</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 2035</v>
       </c>
       <c r="G18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A18</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 2035</v>
       </c>
       <c r="H18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A18</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 2035</v>
       </c>
       <c r="I18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A18</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 2035</v>
       </c>
     </row>
@@ -1037,23 +1052,23 @@
         <v>#REF!</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C19&amp;".xml "&amp;$A19</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 3608</v>
       </c>
       <c r="F19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A19</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 3608</v>
       </c>
       <c r="G19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A19</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 3608</v>
       </c>
       <c r="H19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A19</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 3608</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A19</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 3608</v>
       </c>
     </row>
@@ -1072,23 +1087,23 @@
         <v>#REF!</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C20&amp;".xml "&amp;$A20</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 7716</v>
       </c>
       <c r="F20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A20</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 7716</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A20</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 7716</v>
       </c>
       <c r="H20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A20</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 7716</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A20</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 7716</v>
       </c>
     </row>
@@ -1107,23 +1122,23 @@
         <v>#REF!</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C21&amp;".xml "&amp;$A21</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 5576</v>
       </c>
       <c r="F21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A21</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 5576</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A21</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 5576</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A21</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 5576</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A21</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 5576</v>
       </c>
     </row>
@@ -1142,23 +1157,23 @@
         <v>#REF!</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C22&amp;".xml "&amp;$A22</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 8384</v>
       </c>
       <c r="F22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A22</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 8384</v>
       </c>
       <c r="G22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A22</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 8384</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A22</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 8384</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A22</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 8384</v>
       </c>
     </row>
@@ -1177,23 +1192,23 @@
         <v>#REF!</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C23&amp;".xml "&amp;$A23</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 9968</v>
       </c>
       <c r="F23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A23</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9968</v>
       </c>
       <c r="G23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A23</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9968</v>
       </c>
       <c r="H23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A23</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9968</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A23</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9968</v>
       </c>
     </row>
@@ -1212,23 +1227,23 @@
         <v>#REF!</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C24&amp;".xml "&amp;$A24</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 9288</v>
       </c>
       <c r="F24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A24</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9288</v>
       </c>
       <c r="G24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A24</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9288</v>
       </c>
       <c r="H24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A24</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9288</v>
       </c>
       <c r="I24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A24</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9288</v>
       </c>
     </row>
@@ -1247,23 +1262,23 @@
         <v>#REF!</v>
       </c>
       <c r="E25" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C25&amp;".xml "&amp;$A25</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 7680</v>
       </c>
       <c r="F25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A25</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 7680</v>
       </c>
       <c r="G25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A25</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 7680</v>
       </c>
       <c r="H25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A25</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 7680</v>
       </c>
       <c r="I25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A25</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 7680</v>
       </c>
     </row>
@@ -1282,23 +1297,23 @@
         <v>#REF!</v>
       </c>
       <c r="E26" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C26&amp;".xml "&amp;$A26</f>
+        <f t="shared" si="1"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 10292</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A26</f>
+        <f t="shared" ref="F26:I45" si="3">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A26</f>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10292</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A26</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10292</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A26</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10292</v>
       </c>
       <c r="I26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A26</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10292</v>
       </c>
     </row>
@@ -1314,23 +1329,23 @@
         <v>#REF!</v>
       </c>
       <c r="E27" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C27&amp;".xml "&amp;$A27</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="F27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A27</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A27</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A27</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A27</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1346,23 +1361,23 @@
         <v>#REF!</v>
       </c>
       <c r="E28" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C28&amp;".xml "&amp;$A28</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="F28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A28</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A28</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A28</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A28</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1378,23 +1393,23 @@
         <v>#REF!</v>
       </c>
       <c r="E29" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C29&amp;".xml "&amp;$A29</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="F29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A29</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A29</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A29</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A29</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1410,23 +1425,23 @@
         <v>#REF!</v>
       </c>
       <c r="E30" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C30&amp;".xml "&amp;$A30</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="F30" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A30</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G30" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A30</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H30" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A30</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I30" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A30</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1442,23 +1457,23 @@
         <v>#REF!</v>
       </c>
       <c r="E31" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C31&amp;".xml "&amp;$A31</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="F31" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A31</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G31" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A31</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H31" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A31</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I31" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A31</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1474,23 +1489,23 @@
         <v>#REF!</v>
       </c>
       <c r="E32" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C32&amp;".xml "&amp;$A32</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="F32" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A32</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G32" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A32</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H32" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A32</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I32" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A32</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1506,23 +1521,23 @@
         <v>#REF!</v>
       </c>
       <c r="E33" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C33&amp;".xml "&amp;$A33</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A33</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G33" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A33</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H33" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A33</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I33" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A33</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1538,23 +1553,23 @@
         <v>#REF!</v>
       </c>
       <c r="E34" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C34&amp;".xml "&amp;$A34</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A34</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G34" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A34</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H34" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A34</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I34" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A34</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1570,23 +1585,23 @@
         <v>#REF!</v>
       </c>
       <c r="E35" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C35&amp;".xml "&amp;$A35</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A35</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G35" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A35</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H35" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A35</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I35" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A35</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1602,23 +1617,23 @@
         <v>#REF!</v>
       </c>
       <c r="E36" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C36&amp;".xml "&amp;$A36</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A36</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G36" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A36</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H36" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A36</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I36" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A36</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1634,23 +1649,23 @@
         <v>#REF!</v>
       </c>
       <c r="E37" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C37&amp;".xml "&amp;$A37</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="F37" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A37</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G37" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A37</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H37" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A37</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I37" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A37</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1666,23 +1681,23 @@
         <v>#REF!</v>
       </c>
       <c r="E38" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C38&amp;".xml "&amp;$A38</f>
+        <f t="shared" ref="E38:E60" si="4">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C38&amp;".xml "&amp;$A38</f>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A38</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G38" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A38</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H38" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A38</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I38" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A38</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1698,23 +1713,23 @@
         <v>#REF!</v>
       </c>
       <c r="E39" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C39&amp;".xml "&amp;$A39</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="F39" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A39</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G39" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A39</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H39" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A39</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I39" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A39</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1730,23 +1745,23 @@
         <v>#REF!</v>
       </c>
       <c r="E40" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C40&amp;".xml "&amp;$A40</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A40</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G40" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A40</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H40" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A40</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I40" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A40</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1762,23 +1777,23 @@
         <v>#REF!</v>
       </c>
       <c r="E41" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C41&amp;".xml "&amp;$A41</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="F41" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A41</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G41" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A41</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H41" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A41</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I41" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A41</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1794,23 +1809,23 @@
         <v>#REF!</v>
       </c>
       <c r="E42" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C42&amp;".xml "&amp;$A42</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="F42" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A42</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G42" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A42</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H42" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A42</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I42" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A42</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1826,23 +1841,23 @@
         <v>#REF!</v>
       </c>
       <c r="E43" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C43&amp;".xml "&amp;$A43</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="F43" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A43</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G43" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A43</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H43" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A43</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I43" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A43</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1858,23 +1873,23 @@
         <v>#REF!</v>
       </c>
       <c r="E44" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C44&amp;".xml "&amp;$A44</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="F44" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A44</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G44" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A44</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H44" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A44</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I44" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A44</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1890,23 +1905,23 @@
         <v>#REF!</v>
       </c>
       <c r="E45" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C45&amp;".xml "&amp;$A45</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="F45" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A45</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G45" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A45</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H45" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A45</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I45" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A45</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1922,23 +1937,23 @@
         <v>#REF!</v>
       </c>
       <c r="E46" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C46&amp;".xml "&amp;$A46</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="F46" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A46</f>
+        <f t="shared" ref="F46:I59" si="5">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A46</f>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G46" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A46</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H46" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A46</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I46" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A46</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1954,23 +1969,23 @@
         <v>#REF!</v>
       </c>
       <c r="E47" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C47&amp;".xml "&amp;$A47</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="F47" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A47</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G47" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A47</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H47" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A47</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I47" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A47</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -1986,23 +2001,23 @@
         <v>#REF!</v>
       </c>
       <c r="E48" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C48&amp;".xml "&amp;$A48</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="F48" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A48</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G48" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A48</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H48" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A48</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I48" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A48</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2018,23 +2033,23 @@
         <v>#REF!</v>
       </c>
       <c r="E49" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C49&amp;".xml "&amp;$A49</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="F49" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A49</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G49" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A49</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H49" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A49</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I49" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A49</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2050,23 +2065,23 @@
         <v>#REF!</v>
       </c>
       <c r="E50" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C50&amp;".xml "&amp;$A50</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="F50" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A50</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G50" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A50</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H50" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A50</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I50" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A50</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2082,23 +2097,23 @@
         <v>#REF!</v>
       </c>
       <c r="E51" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C51&amp;".xml "&amp;$A51</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="F51" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A51</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G51" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A51</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H51" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A51</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I51" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A51</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2114,23 +2129,23 @@
         <v>#REF!</v>
       </c>
       <c r="E52" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C52&amp;".xml "&amp;$A52</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="F52" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A52</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G52" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A52</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H52" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A52</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I52" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A52</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2146,23 +2161,23 @@
         <v>#REF!</v>
       </c>
       <c r="E53" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C53&amp;".xml "&amp;$A53</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="F53" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A53</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G53" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A53</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H53" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A53</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I53" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A53</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2178,23 +2193,23 @@
         <v>#REF!</v>
       </c>
       <c r="E54" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C54&amp;".xml "&amp;$A54</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="F54" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A54</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G54" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A54</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H54" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A54</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I54" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A54</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2210,23 +2225,23 @@
         <v>#REF!</v>
       </c>
       <c r="E55" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C55&amp;".xml "&amp;$A55</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="F55" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A55</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G55" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A55</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H55" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A55</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I55" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A55</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2242,23 +2257,23 @@
         <v>#REF!</v>
       </c>
       <c r="E56" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C56&amp;".xml "&amp;$A56</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="F56" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A56</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G56" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A56</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H56" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A56</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I56" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A56</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2274,23 +2289,23 @@
         <v>#REF!</v>
       </c>
       <c r="E57" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C57&amp;".xml "&amp;$A57</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="F57" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A57</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G57" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A57</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H57" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A57</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I57" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A57</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2306,23 +2321,23 @@
         <v>#REF!</v>
       </c>
       <c r="E58" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C58&amp;".xml "&amp;$A58</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="F58" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A58</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G58" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A58</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H58" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A58</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I58" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A58</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2338,23 +2353,23 @@
         <v>#REF!</v>
       </c>
       <c r="E59" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C59&amp;".xml "&amp;$A59</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="F59" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A59</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="G59" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A59</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="H59" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A59</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="I59" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A59</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
@@ -2370,7 +2385,7 @@
         <v>#REF!</v>
       </c>
       <c r="E60" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$C60&amp;".xml "&amp;$A60</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet7.xml </v>
       </c>
     </row>
@@ -2387,10 +2402,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,7 +2414,7 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2473,7 +2488,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3228</v>
+        <v>9044</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -2487,31 +2502,31 @@
       </c>
       <c r="E6" t="str">
         <f>$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;E$4&amp;".xml "&amp;" "&amp;$A6</f>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-0.xml  3228</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-0.xml  9044</v>
       </c>
       <c r="F6" s="4" t="str">
         <f>$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;F$4&amp;".xml "&amp;" "&amp;$A6</f>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-1.xml  3228</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-1.xml  9044</v>
       </c>
       <c r="G6" s="4" t="str">
         <f t="shared" ref="G6:H7" si="0">$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;G$4&amp;".xml "&amp;" "&amp;$A6</f>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-2.xml  3228</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-2.xml  9044</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-3.xml  3228</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-3.xml  9044</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="4" t="str">
         <f>$B$3&amp;" Train "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;C7&amp;".xml "&amp;$B$2&amp;B7&amp;".xml"</f>
-        <v>zzz Train 50 Config/50/Client.xml Config/50/trainDS2.xml Config/50/Engine1.xml</v>
+        <v>zzz Train 50 Config/50/Client.xml Config/50/trainDS2.xml Config/50/Engine2.xml</v>
       </c>
       <c r="E7" s="4" t="str">
         <f>$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;E$4&amp;".xml "&amp;" "&amp;$A7</f>
@@ -2528,6 +2543,26 @@
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-3.xml  </v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MQL5 was saving wrong forecast in db. sEngine Checks shape of infer dataset before proceeding. more tests
</commit_message>
<xml_diff>
--- a/Config/50/TestSet50.xlsx
+++ b/Config/50/TestSet50.xlsx
@@ -97,34 +97,34 @@
     <t>InferDataSet</t>
   </si>
   <si>
-    <t>InferDS1-0</t>
-  </si>
-  <si>
-    <t>InferDS1-1</t>
-  </si>
-  <si>
-    <t>InferDS1-2</t>
-  </si>
-  <si>
-    <t>InferDS1-3</t>
-  </si>
-  <si>
     <t>trainDS2</t>
   </si>
   <si>
-    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-0.xml  9044</t>
-  </si>
-  <si>
-    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-1.xml  9044</t>
-  </si>
-  <si>
-    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-2.xml  9044</t>
-  </si>
-  <si>
-    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-3.xml  9044</t>
-  </si>
-  <si>
     <t>Engine2</t>
+  </si>
+  <si>
+    <t>InferDS2-0</t>
+  </si>
+  <si>
+    <t>InferDS2-1</t>
+  </si>
+  <si>
+    <t>InferDS2-2</t>
+  </si>
+  <si>
+    <t>InferDS2-3</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-0.xml  12932</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-1.xml  12932</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-2.xml  12932</t>
+  </si>
+  <si>
+    <t>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-3.xml  12932</t>
   </si>
 </sst>
 </file>
@@ -2402,10 +2402,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E10" sqref="E10:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,16 +2448,16 @@
         <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2502,27 +2502,30 @@
       </c>
       <c r="E6" t="str">
         <f>$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;E$4&amp;".xml "&amp;" "&amp;$A6</f>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-0.xml  9044</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-0.xml  9044</v>
       </c>
       <c r="F6" s="4" t="str">
         <f>$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;F$4&amp;".xml "&amp;" "&amp;$A6</f>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-1.xml  9044</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-1.xml  9044</v>
       </c>
       <c r="G6" s="4" t="str">
         <f t="shared" ref="G6:H7" si="0">$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;G$4&amp;".xml "&amp;" "&amp;$A6</f>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-2.xml  9044</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-2.xml  9044</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-3.xml  9044</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-3.xml  9044</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12932</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4" t="str">
         <f>$B$3&amp;" Train "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;C7&amp;".xml "&amp;$B$2&amp;B7&amp;".xml"</f>
@@ -2530,39 +2533,39 @@
       </c>
       <c r="E7" s="4" t="str">
         <f>$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;E$4&amp;".xml "&amp;" "&amp;$A7</f>
-        <v xml:space="preserve">zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-0.xml  </v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-0.xml  12932</v>
       </c>
       <c r="F7" s="4" t="str">
         <f>$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;F$4&amp;".xml "&amp;" "&amp;$A7</f>
-        <v xml:space="preserve">zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-1.xml  </v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-1.xml  12932</v>
       </c>
       <c r="G7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-2.xml  </v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-2.xml  12932</v>
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">zzz Infer 50 Config/50/Client.xml Config/50/InferDS1-3.xml  </v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>24</v>
+        <v>zzz Infer 50 Config/50/Client.xml Config/50/InferDS2-3.xml  12932</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>